<commit_message>
product list download and barcode added
</commit_message>
<xml_diff>
--- a/server/resource/excel/ExcelTemplate.xlsx
+++ b/server/resource/excel/ExcelTemplate.xlsx
@@ -1,68 +1,144 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589B4DEA-7031-4E7C-9AA6-DB519C406696}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xujun/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9C784B-D8AA-C24C-A777-FCE1533B6E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="2004" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="920" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="order" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>ID</t>
+    <t>CODE</t>
   </si>
   <si>
-    <t>路由Name</t>
+    <t>PRODUCT NAME</t>
   </si>
   <si>
-    <t>路由Path</t>
+    <t>PACKING</t>
   </si>
   <si>
-    <t>是否隐藏</t>
+    <t>EXP</t>
   </si>
   <si>
-    <t>父节点</t>
+    <t>QTY</t>
   </si>
   <si>
-    <t>排序</t>
-  </si>
-  <si>
-    <t>文件名称</t>
-  </si>
-  <si>
-    <t>https://www.gin-vue-admin.com</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>/</t>
+    <r>
+      <t xml:space="preserve">        S&amp;L FOOD TRADING LTD
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">     10 Merbury Road  London  SE28 0HR</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ [$€-2]* #,##0.00_ ;_ [$€-2]* \-#,##0.00_ ;_ [$€-2]* &quot;-&quot;??_ "/>
+    <numFmt numFmtId="178" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
+    <numFmt numFmtId="179" formatCode="0_);[Red]\(0\)"/>
+  </numFmts>
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -82,16 +158,75 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="12">
+    <cellStyle name="?鹎%U龡&amp;H鼼_x0008__x0001__x001f_?_x0007__x0001__x0001_" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 5" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 5 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="常规 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="常规 4" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="常规 4 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="千位分隔 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="千位分隔 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="样式 1" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color indexed="20"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="45"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -104,8 +239,605 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>723900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5537" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0D790BC-1310-A51F-820D-AD76E34FCBBE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="57150"/>
+          <a:ext cx="876300" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>723900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5538" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1CEA3B8-BE8C-4816-971E-02AA70613DE6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="57150"/>
+          <a:ext cx="917575" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>723900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5539" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D937431-EE64-ABA0-5FE7-2BE5C28CE60F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="57150"/>
+          <a:ext cx="876300" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>14288</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>204788</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>728663</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5540" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80908A05-4462-E041-A4D5-587074C29513}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="14288" y="0"/>
+          <a:ext cx="888371" cy="728663"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>723900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F90B15B5-162E-BA45-8799-9FF822EF81DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="57150"/>
+          <a:ext cx="917575" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>723900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA657897-BD06-8D41-B988-02FF30491C87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="57150"/>
+          <a:ext cx="917575" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>723900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{307E52E7-B020-A44B-A078-7F7B312A4ED3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="57150"/>
+          <a:ext cx="917575" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>14288</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>204788</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>728663</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFEFAA47-8505-7948-99F5-9FF6E32243CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="14288" y="0"/>
+          <a:ext cx="889000" cy="728663"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -121,7 +853,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -133,7 +865,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -180,6 +912,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -215,6 +964,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -357,77 +1123,64 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="52.33203125" defaultRowHeight="30" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="56.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="52.33203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="62.25" customHeight="1">
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="expression" dxfId="0" priority="29" stopIfTrue="1">
+      <formula>AND(COUNTIF($A$1:$A$1, A1)+COUNTIF($A$2:$A$65387, A1)&gt;1,NOT(ISBLANK(A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>